<commit_message>
fix time for thursdays
</commit_message>
<xml_diff>
--- a/div/lectureplan-V26.xlsx
+++ b/div/lectureplan-V26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TECH3\div\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CEFAEE-9FA4-4529-B73C-4F3CC9C1982A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F4A854-2B91-44BD-B17D-BB651BBBF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>Module</t>
   </si>
   <si>
-    <t>Thursday 14:15 - 16:00</t>
-  </si>
-  <si>
     <t>Week</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>16.04: &lt;strong&gt;Oracle session&lt;/strong&gt; in Aud C</t>
+  </si>
+  <si>
+    <t>Thursday 12:15 - 14:00</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,16 +534,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,10 +554,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -565,13 +565,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,10 +582,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,10 +596,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,13 +607,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -624,10 +624,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,10 +638,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,13 +649,13 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,10 +666,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,10 +694,10 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,10 +705,10 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -719,10 +719,10 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -733,10 +733,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -745,17 +745,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2d60b56-d534-48f8-852c-9346ababfcfc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1B0514731AD424F999ECAD5B293E75C" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="791e2903c2d387dd0f8ffbc61bcfe074">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2d60b56-d534-48f8-852c-9346ababfcfc" xmlns:ns3="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79505928d35f7127a600a22198fcd716" ns2:_="" ns3:_="">
     <xsd:import namespace="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
@@ -956,6 +945,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2d60b56-d534-48f8-852c-9346ababfcfc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -966,17 +966,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
-    <ds:schemaRef ds:uri="1a38ecde-d8a6-449a-a4de-d3c0367a81fe"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F9C8970-FADB-48F2-9990-30149F68A38A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -995,6 +984,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
+    <ds:schemaRef ds:uri="1a38ecde-d8a6-449a-a4de-d3c0367a81fe"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
adding datalabs and separate python pages
</commit_message>
<xml_diff>
--- a/div/lectureplan-V26.xlsx
+++ b/div/lectureplan-V26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TECH3\div\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308DA2A8-D033-4754-98D6-136EF08A7FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046441A0-B87F-4121-A78D-169C2AB89F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
   </bookViews>
@@ -116,18 +116,12 @@
     <t>26.02: &lt;strong&gt;Case session 3&lt;/strong&gt;  in Aud J</t>
   </si>
   <si>
-    <t>14.04: &lt;strong&gt;Practical information about exam&lt;/strong&gt; in Aud C</t>
-  </si>
-  <si>
     <t>Tuesday 12:15 -14:00</t>
   </si>
   <si>
     <t>09.04: &lt;strong&gt;Oracle session&lt;/strong&gt; in Aud S</t>
   </si>
   <si>
-    <t>16.04: &lt;strong&gt;Oracle session&lt;/strong&gt; in Aud C</t>
-  </si>
-  <si>
     <t>Thursday 12:15 - 14:00</t>
   </si>
   <si>
@@ -149,7 +143,13 @@
     <t>24.02: &lt;strong&gt;Seminar 2&lt;/strong&gt;  in Aud C.</t>
   </si>
   <si>
-    <t>07.04:  &lt;strong&gt;Seminar 3&lt;/strong&gt; in Aud C</t>
+    <t>16.04: &lt;strong&gt;Practical information about exam&lt;/strong&gt; in Aud C</t>
+  </si>
+  <si>
+    <t>14.04: &lt;strong&gt;Seminar 3&lt;/strong&gt; in Aud C</t>
+  </si>
+  <si>
+    <t>07.04:  &lt;strong&gt;No lecture (oral exams in MAB1)&lt;/strong&gt;</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D0459C-A0F7-4603-AE4B-86A7155DF567}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,10 +537,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -551,7 +551,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -565,7 +565,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -579,7 +579,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -593,10 +593,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
@@ -719,7 +719,7 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,10 +730,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -742,17 +742,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2d60b56-d534-48f8-852c-9346ababfcfc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1B0514731AD424F999ECAD5B293E75C" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="791e2903c2d387dd0f8ffbc61bcfe074">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2d60b56-d534-48f8-852c-9346ababfcfc" xmlns:ns3="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79505928d35f7127a600a22198fcd716" ns2:_="" ns3:_="">
     <xsd:import namespace="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
@@ -953,6 +942,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2d60b56-d534-48f8-852c-9346ababfcfc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -963,17 +963,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
-    <ds:schemaRef ds:uri="1a38ecde-d8a6-449a-a4de-d3c0367a81fe"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F9C8970-FADB-48F2-9990-30149F68A38A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -992,6 +981,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
+    <ds:schemaRef ds:uri="1a38ecde-d8a6-449a-a4de-d3c0367a81fe"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
from Aud S to Aud Q
</commit_message>
<xml_diff>
--- a/div/lectureplan-V26.xlsx
+++ b/div/lectureplan-V26.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TECH3\div\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046441A0-B87F-4121-A78D-169C2AB89F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EA9BD1-6932-4852-A81E-A59B7B092774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15345" xr2:uid="{904F4144-1937-4711-AEEF-991D1AD6F23A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,15 +68,6 @@
     <t>22.01: &lt;strong&gt;Case session 1&lt;/strong&gt; in Aud S</t>
   </si>
   <si>
-    <t>29.01: &lt;strong&gt;Collaborative learning session 2&lt;/strong&gt; in Aud S</t>
-  </si>
-  <si>
-    <t>12.02: &lt;strong&gt;Case session 2&lt;/strong&gt; in Aud S</t>
-  </si>
-  <si>
-    <t>19.02: &lt;strong&gt;Collaborative learning session 3&lt;/strong&gt; in Aud S</t>
-  </si>
-  <si>
     <t>Module 1/2</t>
   </si>
   <si>
@@ -113,9 +104,6 @@
     <t>03.03: &lt;strong&gt;Overview lecture 4&lt;/strong&gt; in Aud C</t>
   </si>
   <si>
-    <t>26.02: &lt;strong&gt;Case session 3&lt;/strong&gt;  in Aud J</t>
-  </si>
-  <si>
     <t>Tuesday 12:15 -14:00</t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t>13.01: &lt;strong&gt;Introduction to TECH3/Overview lecture 1&lt;/strong&gt; in Aud C</t>
   </si>
   <si>
-    <t>05.02: &lt;strong&gt;Exercise session 2&lt;/strong&gt; in Aud S</t>
-  </si>
-  <si>
     <t>03.02: &lt;strong&gt;Seminar 1&lt;/strong&gt; in Aud C</t>
   </si>
   <si>
@@ -150,6 +135,21 @@
   </si>
   <si>
     <t>07.04:  &lt;strong&gt;No lecture (oral exams in MAB1)&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>29.01: &lt;strong&gt;Collaborative learning session 2&lt;/strong&gt; in Aud Q</t>
+  </si>
+  <si>
+    <t>05.02: &lt;strong&gt;Exercise session 2&lt;/strong&gt; in Aud Q</t>
+  </si>
+  <si>
+    <t>12.02: &lt;strong&gt;Case session 2&lt;/strong&gt; in Aud Q</t>
+  </si>
+  <si>
+    <t>19.02: &lt;strong&gt;Collaborative learning session 3&lt;/strong&gt; in Aud Q</t>
+  </si>
+  <si>
+    <t>26.02: &lt;strong&gt;Case session 3&lt;/strong&gt;  in Aud Q</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D0459C-A0F7-4603-AE4B-86A7155DF567}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,10 +537,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -551,7 +551,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -562,10 +562,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -579,10 +579,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -593,10 +593,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -604,13 +604,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,10 +621,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,10 +635,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,10 +649,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,10 +663,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,10 +677,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -716,10 +716,10 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -730,10 +730,10 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -742,6 +742,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2d60b56-d534-48f8-852c-9346ababfcfc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1B0514731AD424F999ECAD5B293E75C" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="791e2903c2d387dd0f8ffbc61bcfe074">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2d60b56-d534-48f8-852c-9346ababfcfc" xmlns:ns3="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79505928d35f7127a600a22198fcd716" ns2:_="" ns3:_="">
     <xsd:import namespace="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
@@ -942,17 +953,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2d60b56-d534-48f8-852c-9346ababfcfc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1a38ecde-d8a6-449a-a4de-d3c0367a81fe" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -963,6 +963,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
+    <ds:schemaRef ds:uri="1a38ecde-d8a6-449a-a4de-d3c0367a81fe"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F9C8970-FADB-48F2-9990-30149F68A38A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -981,17 +992,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EFB0A27-11D7-4D56-8C6B-24FBD61760D5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e2d60b56-d534-48f8-852c-9346ababfcfc"/>
-    <ds:schemaRef ds:uri="1a38ecde-d8a6-449a-a4de-d3c0367a81fe"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62C2037A-10DD-4192-8BFC-ED508F316DB7}">
   <ds:schemaRefs>

</xml_diff>